<commit_message>
Added week 1 notes for teams 4,5, and 7
</commit_message>
<xml_diff>
--- a/Syllabus/ProjectFiles/Teams.xlsx
+++ b/Syllabus/ProjectFiles/Teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t xml:space="preserve">Team #</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t xml:space="preserve">Our dataset needs authorization from a hospital and we are currently in the process of getting it done from a doctor in India. We shall update you once we are ready with the it, but we have the data in hand, but in a pdf file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team has data from 200 patients, received from a doctor in India. Once the team gets approval to use the dataset, they will remove personal identifiers from this dataset. They also plan on generating synthetic dataset to add the dataset, since the current dataset does not contain any stats on healthy patients. The team will then normalize the dataset too.</t>
   </si>
   <si>
     <t xml:space="preserve">ak3328@g.rit.edu</t>
@@ -186,6 +189,9 @@
     <t xml:space="preserve">https://grouplens.org/datasets/movielens/tag-genome/</t>
   </si>
   <si>
+    <t xml:space="preserve">The team has the MovieLens dataset in the form of 3 large “.dat” files, which they have merged into a single “.csv” file. The team has almost finished pre-processing the data and is currently performing EDA. As the EDA phase progresses, the final research question asked in this project might change as the team discovers new findings.</t>
+  </si>
+  <si>
     <t xml:space="preserve">av8920@g.rit.edu</t>
   </si>
   <si>
@@ -218,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">Provided by AHRT Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current dataset received by the team is inadequate for a ML project. So, the team is actively seeking a new dataset.</t>
   </si>
 </sst>
 </file>
@@ -468,14 +477,14 @@
   </sheetPr>
   <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.67"/>
@@ -485,7 +494,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="61.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="69.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="10.83"/>
   </cols>
   <sheetData>
@@ -629,7 +638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="170" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="n">
         <v>4</v>
       </c>
@@ -660,8 +669,11 @@
       <c r="K6" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="119" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="n">
         <v>5</v>
       </c>
@@ -672,25 +684,28 @@
         <v>44496.8662152778</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,28 +719,28 @@
         <v>44497.3393518518</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="n">
         <v>7</v>
       </c>
@@ -736,25 +751,28 @@
         <v>44497.7744791667</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added week 2 notes for teams 1-3
</commit_message>
<xml_diff>
--- a/Syllabus/ProjectFiles/Teams.xlsx
+++ b/Syllabus/ProjectFiles/Teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t xml:space="preserve">Team #</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Week 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Week 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">11/02, 11/09, 11/16, 11/23</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">The team is using very old data. And, they have found a few issues with this dataset. There is a class imbalance problem because 80% of the data is just about attacks. They are adding 14 new target labels to the testing dataset and planning to drop incorrect labels in the training dataset. They are working on pre-processing the data further.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team is using 10% of the data to be able to fit their model on their local machine. They have added synthetic data that represents non-DDOS attacks, because the original dataset is highly imbalanced. They are now starting to use use ML models like unsupervised clustering classification models.</t>
   </si>
   <si>
     <t xml:space="preserve">ln8378@g.rit.edu</t>
@@ -106,6 +112,9 @@
     <t xml:space="preserve">The team has scraped the data from a public government website using Selenium. They have performed some pre-processing on the data, including fixing an issue where states with two words in their names were showing up as separate entries. They now have a dataset with many features. So, they are performing EDA and exploring ways to convert these large number of columns into a feature space that can be fed into a model.</t>
   </si>
   <si>
+    <t xml:space="preserve">The team has started with the EDA phase. They are working on finding congressman that have voted against their party for each bill right now. A few issues with visualization were discussed and the team will try out some suggested solutions. The team is manually reviewing the data as well to find bills that represent high polarity, in order to perform a deeper analysis on such bills. The are looking to gain insights from such bills to see how the congressman vote on particular issues.</t>
+  </si>
+  <si>
     <t xml:space="preserve">pn1922@g.rit.edu</t>
   </si>
   <si>
@@ -123,13 +132,16 @@
   </si>
   <si>
     <t xml:space="preserve">We plan to divide every task like data cleaning, EDA, feature engineering, model training and testing equally among the four of us.
-Since the training data contains 200,000 rows, one person handling a single task in one computer can be challenging in terms of computation. Hence, we plan to split every task equally amongst us</t>
+Since the training data contains 200,000 rows, one person handling a single task in one computer can be challenging in terms of computation. Hence, we plan to split every task equally among us</t>
   </si>
   <si>
     <t xml:space="preserve">https://he-s3.s3.amazonaws.com/media/hackathon/machine-learning-indiahacks-2017/5f828822-4--4-hotstar_dataset.zip</t>
   </si>
   <si>
     <t xml:space="preserve">The team has separate per-city and per-time-of-day watch times, which they have pre-processed into separate columns. Instead of pre-processing in memory, they have applied pre-processing in batches on the data. They are now performing EDA on the separate pieces of the dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the dataset, some genres and cities have more NaNs than others. So, the features with low number of NaNs will be handled separately from the features with higher number of NaNs. They performed clustering with the features that they had and could not find meaningful insights due to the large number of features. So, the team will perform dimensionality reduction and pick the top dimensions based on their representation of variance in the data, in order to assist the underlying clustering algorithm. The team is thinking of running two models: One that takes just the "watch time" to predict the "time" when the customer will log in again, and the second one where clustering is used to find genres to suggest based on similar genres in the cities of the customers.</t>
   </si>
   <si>
     <t xml:space="preserve">11/04,11/11,11/18,11/30</t>
@@ -475,10 +487,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:L9"/>
+  <dimension ref="B2:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,10 +507,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="61.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="69.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="32.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -531,6 +544,9 @@
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="135.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -538,34 +554,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>44495.6291319444</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -573,69 +592,75 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>44495.6498611111</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="252.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>44495.7207523148</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,34 +668,34 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>44496.0786111111</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,34 +703,34 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>44496.8662152778</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,31 +738,31 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>44497.3393518518</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,34 +770,34 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="8" t="n">
         <v>44497.7744791667</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added week 3 notes for teams 1-3
</commit_message>
<xml_diff>
--- a/Syllabus/ProjectFiles/Teams.xlsx
+++ b/Syllabus/ProjectFiles/Teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t xml:space="preserve">Team #</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Week 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Week 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">11/02, 11/09, 11/16, 11/23</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">The team is using 10% of the data to be able to fit their model on their local machine. They have added synthetic data that represents non-DDOS attacks, because the original dataset is highly imbalanced. They are now starting to use use ML models like unsupervised clustering classification models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team is using 10% over their dataset for now. They are using oversampling technique to handle the class imbalance issue. They have used one-hot encoder for categorical data. They have tried Decision Tree and Naive Bayes until now. They are working on more models. Since there is high correlation between some columns, the team is planning to test dimensionality reduction.</t>
   </si>
   <si>
     <t xml:space="preserve">ln8378@g.rit.edu</t>
@@ -115,6 +121,9 @@
     <t xml:space="preserve">The team has started with the EDA phase. They are working on finding congressman that have voted against their party for each bill right now. A few issues with visualization were discussed and the team will try out some suggested solutions. The team is manually reviewing the data as well to find bills that represent high polarity, in order to perform a deeper analysis on such bills. The are looking to gain insights from such bills to see how the congressman vote on particular issues.</t>
   </si>
   <si>
+    <t xml:space="preserve">The team has performed some more EDA to try to separate the distribution of votes per party.</t>
+  </si>
+  <si>
     <t xml:space="preserve">pn1922@g.rit.edu</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">In the dataset, some genres and cities have more NaNs than others. So, the features with low number of NaNs will be handled separately from the features with higher number of NaNs. They performed clustering with the features that they had and could not find meaningful insights due to the large number of features. So, the team will perform dimensionality reduction and pick the top dimensions based on their representation of variance in the data, in order to assist the underlying clustering algorithm. The team is thinking of running two models: One that takes just the "watch time" to predict the "time" when the customer will log in again, and the second one where clustering is used to find genres to suggest based on similar genres in the cities of the customers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After separating the “dow”, “cities”, and “genres” columns, the team got a very large number of features. The team realized that the total time is the same for “dow”, “cities”, and “genres”. So, the team decided to go only with the “dow” column. They have used Logistic Regression but it doesn't perform well. So, they are trying out different feature engineering techniques now.</t>
   </si>
   <si>
     <t xml:space="preserve">11/04,11/11,11/18,11/30</t>
@@ -239,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">The current dataset received by the team is inadequate for a ML project. So, the team is actively seeking a new dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since the previous dataset didn’t have enough information to be used in a Data Science project, the team has obtained a new dataset about NYC AirBnB prices. They are currently preprocessing the dataset and will move on to EDA after this part.</t>
   </si>
 </sst>
 </file>
@@ -487,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:M9"/>
+  <dimension ref="B2:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,8 +522,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="61.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="69.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="32.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="32.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,43 +564,49 @@
       <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="135.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>44495.6291319444</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -592,37 +614,40 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>44495.6498611111</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="252.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,37 +655,40 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>44495.7207523148</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,34 +696,34 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>44496.0786111111</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,34 +731,34 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>44496.8662152778</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,66 +766,69 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>44497.3393518518</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="n">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D9" s="8" t="n">
         <v>44497.7744791667</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added week 3 notes for teams 4-7
</commit_message>
<xml_diff>
--- a/Syllabus/ProjectFiles/Teams.xlsx
+++ b/Syllabus/ProjectFiles/Teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t xml:space="preserve">Team #</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">The team has data from 200 patients, received from a doctor in India. Once the team gets approval to use the dataset, they will remove personal identifiers from this dataset. They also plan on generating synthetic dataset to add the dataset, since the current dataset does not contain any stats on healthy patients. The team will then normalize the dataset too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team has investigated various datasets and methods currently used in research. The team has permission to use these datasets for research. So, they are currently working on exploratory data analysis on these datasets to decide which one to use.</t>
   </si>
   <si>
     <t xml:space="preserve">ak3328@g.rit.edu</t>
@@ -216,6 +219,9 @@
     <t xml:space="preserve">The team has the MovieLens dataset in the form of 3 large “.dat” files, which they have merged into a single “.csv” file. The team has almost finished pre-processing the data and is currently performing EDA. As the EDA phase progresses, the final research question asked in this project might change as the team discovers new findings.</t>
   </si>
   <si>
+    <t xml:space="preserve">Data analysis has been completed. The team is working on the KNN model. They are also checking to see if they can use any other clustering technique or augment their dataset using summaries of movie from a different data source.</t>
+  </si>
+  <si>
     <t xml:space="preserve">av8920@g.rit.edu</t>
   </si>
   <si>
@@ -229,6 +235,9 @@
   </si>
   <si>
     <t xml:space="preserve">Will be Provided by instructor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data pre-processing has been started. Random Forest and Stacked Classifier model is being planned.</t>
   </si>
   <si>
     <t xml:space="preserve">nk1976@g.rit.edu</t>
@@ -254,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">Since the previous dataset didn’t have enough information to be used in a Data Science project, the team has obtained a new dataset about NYC AirBnB prices. They are currently preprocessing the dataset and will move on to EDA after this part.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data pre-processing has been completed. The team is currently in the exploratory data analysis and feature engineering phase.</t>
   </si>
 </sst>
 </file>
@@ -504,8 +516,8 @@
   </sheetPr>
   <dimension ref="B2:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,6 +737,9 @@
       <c r="L6" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="n">
@@ -737,31 +752,34 @@
         <v>44496.8662152778</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="n">
         <v>6</v>
       </c>
@@ -772,25 +790,28 @@
         <v>44497.3393518518</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,31 +825,34 @@
         <v>44497.7744791667</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added week 4 notes for teams 1-3, 5, and 7
</commit_message>
<xml_diff>
--- a/Syllabus/ProjectFiles/Teams.xlsx
+++ b/Syllabus/ProjectFiles/Teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t xml:space="preserve">Team #</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Week 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Week 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">11/02, 11/09, 11/16, 11/23</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">The team is using 10% over their dataset for now. They are using oversampling technique to handle the class imbalance issue. They have used one-hot encoder for categorical data. They have tried Decision Tree and Naive Bayes until now. They are working on more models. Since there is high correlation between some columns, the team is planning to test dimensionality reduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team has tested over-sampling and under-sampling and they are getting a very high F1 score and accuracy. So, it's possible that the model is over-fitting. They are investigating to see what could be the problem here.</t>
   </si>
   <si>
     <t xml:space="preserve">ln8378@g.rit.edu</t>
@@ -124,6 +130,9 @@
     <t xml:space="preserve">The team has performed some more EDA to try to separate the distribution of votes per party.</t>
   </si>
   <si>
+    <t xml:space="preserve">The team is working on using cosine similarity and Jaccard similarity coefficient to find politicians with similar voting patterns.</t>
+  </si>
+  <si>
     <t xml:space="preserve">pn1922@g.rit.edu</t>
   </si>
   <si>
@@ -154,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">After separating the “dow”, “cities”, and “genres” columns, the team got a very large number of features. The team realized that the total time is the same for “dow”, “cities”, and “genres”. So, the team decided to go only with the “dow” column. They have used Logistic Regression but it doesn't perform well. So, they are trying out different feature engineering techniques now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team has tried various models and getting very low scores ROC-AUC scores. So, they are performing more feature engineering to get better results from the dataset.</t>
   </si>
   <si>
     <t xml:space="preserve">11/04,11/11,11/18,11/30</t>
@@ -222,6 +234,9 @@
     <t xml:space="preserve">Data analysis has been completed. The team is working on the KNN model. They are also checking to see if they can use any other clustering technique or augment their dataset using summaries of movie from a different data source.</t>
   </si>
   <si>
+    <t xml:space="preserve">The team has used cosine similarity on TF-IDF vectors to find similar movies for their recommendation system. The next step will be collaborative filtering in their project. The team is brainstorming ways to validate the goodness of fit for these recommendations.</t>
+  </si>
+  <si>
     <t xml:space="preserve">av8920@g.rit.edu</t>
   </si>
   <si>
@@ -266,6 +281,9 @@
   </si>
   <si>
     <t xml:space="preserve">Data pre-processing has been completed. The team is currently in the exploratory data analysis and feature engineering phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team has been working through outliers in their dataset. They are now working on their ML models.</t>
   </si>
 </sst>
 </file>
@@ -514,10 +532,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:N9"/>
+  <dimension ref="B2:O9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -536,7 +554,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="32.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="32.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,46 +598,52 @@
       <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="135.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>44495.6291319444</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="4" t="n">
         <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -626,40 +651,43 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>44495.6498611111</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="252.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,40 +695,43 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>44495.7207523148</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,37 +739,37 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>44496.0786111111</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,37 +777,40 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>44496.8662152778</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,34 +818,34 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>44497.3393518518</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,40 +853,43 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D9" s="8" t="n">
         <v>44497.7744791667</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>